<commit_message>
small fixes for training pipeline
</commit_message>
<xml_diff>
--- a/compliance/risk_register.xlsx
+++ b/compliance/risk_register.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,6 +448,48 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>53db1b10-3d9a-4d9b-93d6-bb719553e342</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5649999999999999</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Mitigation needed</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>6f7e2563-4400-4e4b-9f39-02b0ea2de25a</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5649999999999999</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Mitigation needed</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor and add additional artifacts
</commit_message>
<xml_diff>
--- a/compliance/risk_register.xlsx
+++ b/compliance/risk_register.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,6 +490,27 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>99aa059c-c144-4966-bbca-95917aa70b10</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.5649999999999999</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Mitigation needed</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor and complete modal deployment template
</commit_message>
<xml_diff>
--- a/compliance/risk_register.xlsx
+++ b/compliance/risk_register.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +511,27 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>74d68dde-c792-4fdf-8cea-0a6960ef2e5c</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.465</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Mitigation needed</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>